<commit_message>
added another calculated column
</commit_message>
<xml_diff>
--- a/Master Submitted Log New.xlsx
+++ b/Master Submitted Log New.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -31,10 +31,16 @@
     <t>Word</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Amazon</t>
   </si>
   <si>
     <t>word</t>
+  </si>
+  <si>
+    <t>KL-OLW-LIKE</t>
   </si>
   <si>
     <t>Google</t>
@@ -43,7 +49,13 @@
     <t>Facebook</t>
   </si>
   <si>
+    <t>HU-WE-LIKE</t>
+  </si>
+  <si>
     <t>Youtube</t>
+  </si>
+  <si>
+    <t>JT-LSK-LIKE</t>
   </si>
 </sst>
 </file>
@@ -52,10 +64,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -77,14 +89,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -105,9 +131,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,16 +170,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,85 +233,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,7 +248,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,19 +380,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,91 +398,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,49 +422,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,6 +451,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -450,15 +471,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,6 +491,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -493,17 +520,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,150 +539,127 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -668,10 +668,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -945,13 +957,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.71428571428571" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
@@ -961,7 +973,7 @@
     <col min="6" max="6" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" ht="12.75" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -978,10 +990,13 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="12.75" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3">
         <v>43836</v>
@@ -994,12 +1009,15 @@
         <v>43838</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>43836</v>
@@ -1012,12 +1030,15 @@
         <v>43838</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>43836</v>
@@ -1030,12 +1051,15 @@
         <v>43839</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>43838</v>
@@ -1048,12 +1072,15 @@
         <v>43840</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" spans="1:8">
+      <c r="A6" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>43839</v>
@@ -1066,12 +1093,15 @@
         <v>43840</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>43840</v>
@@ -1084,12 +1114,15 @@
         <v>43841</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
         <v>43840</v>
@@ -1102,12 +1135,15 @@
         <v>43844</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <v>43840</v>
@@ -1120,10 +1156,13 @@
         <v>43844</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" spans="2:5">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>

</xml_diff>